<commit_message>
Modify and add more replacements
</commit_message>
<xml_diff>
--- a/Stellaris Theme Project Manager.xlsx
+++ b/Stellaris Theme Project Manager.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="186">
   <si>
     <t>需求名</t>
   </si>
@@ -186,7 +186,7 @@
     <t>光标</t>
   </si>
   <si>
-    <t>有毛边（后续迭代）</t>
+    <t>待验证</t>
   </si>
   <si>
     <t>允许尺寸超过原素材</t>
@@ -201,9 +201,6 @@
     <t>按钮不完全占满时出现的背景填充色</t>
   </si>
   <si>
-    <t>待验证</t>
-  </si>
-  <si>
     <t>测试修改为透明</t>
   </si>
   <si>
@@ -345,9 +342,6 @@
     <t>完全禁用</t>
   </si>
   <si>
-    <t>区分度较低</t>
-  </si>
-  <si>
     <t>会以缩放形式复用至右下角叠加层的开关，如果制作外框则视效不佳</t>
   </si>
   <si>
@@ -438,9 +432,6 @@
     <t>订单窗口右上角-前一个</t>
   </si>
   <si>
-    <t>新增</t>
-  </si>
-  <si>
     <t>待验证，可能通过翻转使用，鼠标悬停时会变暗</t>
   </si>
   <si>
@@ -493,6 +484,9 @@
   </si>
   <si>
     <t>订单减少</t>
+  </si>
+  <si>
+    <t>可能会被缩放使用，不建议制作外框</t>
   </si>
   <si>
     <t>TexButton.Plus</t>
@@ -592,7 +586,7 @@
     <numFmt numFmtId="177" formatCode="_ \￥* #,##0_ ;_ \￥* \-#,##0_ ;_ \￥* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,13 +602,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7"/>
-      <name val="等线"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="9"/>
       <name val="等线"/>
       <charset val="134"/>
     </font>
@@ -625,13 +613,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="7"/>
       <name val="等线"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9"/>
+      <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
     </font>
@@ -1171,7 +1159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1189,134 +1177,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1365,6 +1353,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1386,6 +1377,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1398,15 +1392,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1430,9 +1415,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1824,436 +1806,436 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="41" t="s">
+      <c r="E2" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="41" t="s">
+      <c r="E3" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="41" t="s">
+      <c r="E4" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="41" t="s">
+      <c r="E5" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="41" t="s">
+      <c r="E6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="41" t="s">
+      <c r="E7" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="41" t="s">
+      <c r="E8" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="41" t="s">
+      <c r="E9" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="41" t="s">
+      <c r="E10" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="41" t="s">
+      <c r="E11" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="41" t="s">
+      <c r="E12" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="41" t="s">
+      <c r="E13" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="41" t="s">
+      <c r="E14" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="41" t="s">
+      <c r="E15" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="41" t="s">
+      <c r="E16" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="41" t="s">
+      <c r="E17" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="41" t="s">
+      <c r="E18" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="44" t="s">
+      <c r="E19" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="42" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="45"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="46"/>
+      <c r="F20" s="44"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="45"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="46"/>
+      <c r="F21" s="44"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="45"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="46"/>
+      <c r="F22" s="44"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="45"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="46"/>
+      <c r="F23" s="44"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="45"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="46"/>
+      <c r="F24" s="44"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="45"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="46"/>
+      <c r="F25" s="44"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="45"/>
+      <c r="A26" s="43"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="46"/>
+      <c r="F26" s="44"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="45"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="46"/>
+      <c r="F27" s="44"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="47"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="48"/>
+      <c r="D28" s="46"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="49"/>
+      <c r="F28" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2266,10 +2248,10 @@
   <sheetPr/>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -2338,114 +2320,114 @@
       <c r="E3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>61</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="16" t="s">
+      <c r="B6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="19" t="s">
+      <c r="B7" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="E7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="19" t="s">
+      <c r="B8" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="19" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>10</v>
@@ -2454,16 +2436,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>78</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>10</v>
@@ -2472,16 +2454,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>80</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>10</v>
@@ -2490,16 +2472,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>82</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>10</v>
@@ -2508,88 +2490,88 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="E13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="E14" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="19" t="s">
+      <c r="B15" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="20" t="s">
+      <c r="E15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="19" t="s">
+      <c r="D16" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="19" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>94</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>10</v>
@@ -2598,479 +2580,483 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="E18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="23" t="s">
         <v>97</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="19" t="s">
+      <c r="B20" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="21" t="s">
+      <c r="E20" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="F20" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="6" t="s">
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="17" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="19" t="s">
+      <c r="B21" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="21" t="s">
+      <c r="E21" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" ht="28.5" spans="1:6">
+      <c r="A22" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" ht="28.5" spans="1:6">
-      <c r="A22" s="16" t="s">
+      <c r="B22" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="18" t="s">
+      <c r="E22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="E22" s="18" t="s">
+    </row>
+    <row r="23" ht="28.5" spans="1:6">
+      <c r="A23" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="B23" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="23" ht="28.5" spans="1:6">
-      <c r="A23" s="19" t="s">
+      <c r="E23" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" ht="28.5" spans="1:6">
+      <c r="A24" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="21" t="s">
+      <c r="B24" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" ht="28.5" spans="1:6">
-      <c r="A24" s="19" t="s">
+      <c r="E24" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B24" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="21" t="s">
+      <c r="B25" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="24" t="s">
+      <c r="E25" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="26" t="s">
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="B26" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="24" t="s">
+      <c r="E26" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="26" t="s">
+      <c r="B27" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="E26" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="24" t="s">
+      <c r="E27" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="26" t="s">
+      <c r="B28" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="24" t="s">
+      <c r="E28" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="26" t="s">
+      <c r="B29" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="19" t="s">
+      <c r="E29" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" s="21" t="s">
+      <c r="B30" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="24" t="s">
+      <c r="E30" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B30" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" s="26" t="s">
+      <c r="B31" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="13" t="s">
+      <c r="E31" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="15" t="s">
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="B32" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="13" t="s">
+      <c r="E32" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="15" t="s">
+      <c r="B33" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="27" t="s">
+      <c r="E33" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="29" t="s">
+      <c r="B34" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="E33" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="30" t="s">
+      <c r="E34" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="32" t="s">
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="E34" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="F34" s="33" t="s">
+      <c r="B35" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="34" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="34" t="s">
+      <c r="E35" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="35" t="s">
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="B36" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="E36" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="33" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="34" t="s">
+      <c r="B37" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="35" t="s">
+      <c r="D37" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="E36" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="F36" s="34" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="34" t="s">
+      <c r="E37" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="B37" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="34" t="s">
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="B38" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="E37" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="F37" s="34" t="s">
+      <c r="E38" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="34" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="34" t="s">
+    <row r="39" spans="1:6">
+      <c r="A39" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="35" t="s">
+      <c r="B39" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="F38" s="35" t="s">
+      <c r="E39" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="35" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="34" t="s">
+      <c r="B40" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="B39" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="35" t="s">
+      <c r="E40" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="E39" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="F39" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="36" t="s">
+      <c r="F40" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="B40" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="37" t="s">
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="E40" s="37" t="s">
+      <c r="B41" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="F40" s="36" t="s">
+      <c r="E41" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="33" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="34" t="s">
+    <row r="42" spans="1:6">
+      <c r="A42" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="B41" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D41" s="35" t="s">
+      <c r="B42" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="E41" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="F41" s="38"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="E42" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="F42" s="38"/>
+      <c r="E42" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F42" s="33" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3097,121 +3083,121 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -3219,7 +3205,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3227,7 +3213,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3235,7 +3221,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>

</xml_diff>

<commit_message>
Add some English descriptions
</commit_message>
<xml_diff>
--- a/Stellaris Theme Project Manager.xlsx
+++ b/Stellaris Theme Project Manager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23835" windowHeight="14310" activeTab="1"/>
+    <workbookView windowWidth="24075" windowHeight="14895" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BGM and SE" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="219">
   <si>
     <t>需求名</t>
   </si>
@@ -162,6 +162,24 @@
     <t>主界面音乐</t>
   </si>
   <si>
+    <t>需求名 defName</t>
+  </si>
+  <si>
+    <t>路径 Path</t>
+  </si>
+  <si>
+    <t>类型 Type</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>进度 Progress</t>
+  </si>
+  <si>
+    <t>备注 Note</t>
+  </si>
+  <si>
     <t>ActiveTip.TooltipBGAtlas</t>
   </si>
   <si>
@@ -174,7 +192,10 @@
     <t>鼠标停驻时出现的工具条</t>
   </si>
   <si>
-    <t>透明度不可用</t>
+    <t>Tooltip window frame when mouse on a pawn, animal, item or context</t>
+  </si>
+  <si>
+    <t>透明度不可用 Transparency not avaliable</t>
   </si>
   <si>
     <t>CustomCursor.CursorTex</t>
@@ -186,7 +207,10 @@
     <t>光标</t>
   </si>
   <si>
-    <t>允许尺寸超过原素材</t>
+    <t>Just mouse</t>
+  </si>
+  <si>
+    <t>允许尺寸超过原素材 allow exceed max size of original texture</t>
   </si>
   <si>
     <t>InspectPaneUtility.InspectTabButtonFillTex</t>
@@ -198,7 +222,10 @@
     <t>按钮不完全占满时出现的背景填充色</t>
   </si>
   <si>
-    <t>测试修改为透明</t>
+    <t>Background fill color that appears when the button is not fully occupied</t>
+  </si>
+  <si>
+    <t>Can be transparent</t>
   </si>
   <si>
     <t>MainMenuDrawer.TexTitle</t>
@@ -210,6 +237,9 @@
     <t>标题界面的标题</t>
   </si>
   <si>
+    <t>main menu title picture</t>
+  </si>
+  <si>
     <t>TabRecord.TabAtlas</t>
   </si>
   <si>
@@ -219,6 +249,9 @@
     <t>标签页</t>
   </si>
   <si>
+    <t>tab</t>
+  </si>
+  <si>
     <t>待验证</t>
   </si>
   <si>
@@ -231,12 +264,18 @@
     <t>标题界面的背景</t>
   </si>
   <si>
+    <t>main menu background</t>
+  </si>
+  <si>
     <t>Widgets.ButtonBarTex</t>
   </si>
   <si>
     <t>底层按钮叠加进度层</t>
   </si>
   <si>
+    <t>Bottom button overlay progress layer, research progress, RuntimeGC mem status, etc</t>
+  </si>
+  <si>
     <t>Widgets.ButtonBGAtlas</t>
   </si>
   <si>
@@ -246,24 +285,36 @@
     <t>通用按钮默认状态</t>
   </si>
   <si>
+    <t>Common button not interactive</t>
+  </si>
+  <si>
     <t>Widgets.ButtonBGAtlasClick</t>
   </si>
   <si>
     <t>通用按钮点击摁住状态</t>
   </si>
   <si>
+    <t>Common button click, click hold</t>
+  </si>
+  <si>
     <t>Widgets.ButtonBGAtlasMouseover</t>
   </si>
   <si>
     <t>通用按钮鼠标划过状态</t>
   </si>
   <si>
+    <t>Common button mouseover, highlight</t>
+  </si>
+  <si>
     <t>Widgets.ButtonSubtleAtlas</t>
   </si>
   <si>
     <t>游戏底部按钮</t>
   </si>
   <si>
+    <t>bottom button, for example, building, research etc</t>
+  </si>
+  <si>
     <t>BGLoader</t>
   </si>
   <si>
@@ -273,9 +324,15 @@
     <t>加载画面的背景</t>
   </si>
   <si>
+    <t>loading pic</t>
+  </si>
+  <si>
     <t>加载画面中央的旋转组件</t>
   </si>
   <si>
+    <t>rotating gizmo in loading</t>
+  </si>
+  <si>
     <t>可以替换（后续迭代）</t>
   </si>
   <si>
@@ -285,12 +342,18 @@
     <t>进度条进度颜色配置</t>
   </si>
   <si>
+    <t>loading interface, loading progress</t>
+  </si>
+  <si>
     <t>TextBar</t>
   </si>
   <si>
     <t>进度条底层颜色配置</t>
   </si>
   <si>
+    <t>loading interface, loading text desc</t>
+  </si>
+  <si>
     <t>Icon</t>
   </si>
   <si>
@@ -300,6 +363,9 @@
     <t>RimThemes 主题按钮</t>
   </si>
   <si>
+    <t>RimThems button</t>
+  </si>
+  <si>
     <t>Tapestry</t>
   </si>
   <si>
@@ -309,7 +375,11 @@
     <t>通用窗口背景板，游戏内自带描边</t>
   </si>
   <si>
-    <t>游戏内会被不保持横纵比例放缩，因而不建议添加纹理</t>
+    <t>common window frame background</t>
+  </si>
+  <si>
+    <t>游戏内会被不保持横纵比例放缩，因而不建议添加纹理
+Drawing textures are not recommended because the game is scaled not keeping horizontally or vertically ratio.</t>
   </si>
   <si>
     <t>Command.BGTex</t>
@@ -318,16 +388,23 @@
     <t>命令按钮通用底层</t>
   </si>
   <si>
+    <t>pawns or utilities command background</t>
+  </si>
+  <si>
     <t>Widgets.RadioButOffTex</t>
   </si>
   <si>
     <t>圆圈选项关闭</t>
   </si>
   <si>
+    <t>radio button, off</t>
+  </si>
+  <si>
     <t>可容忍</t>
   </si>
   <si>
-    <t>游戏内会被缩放使用，修改样式可能导致视效不佳</t>
+    <t>游戏内会被缩放使用，修改样式可能导致视效不佳
+In game it would be used in scaled down, modifying the style may result in poor viewing</t>
   </si>
   <si>
     <t>Widgets.RadioButOnTex</t>
@@ -336,52 +413,41 @@
     <t>圆圈选项启用</t>
   </si>
   <si>
+    <t>radio button, on</t>
+  </si>
+  <si>
     <t>Widgets.CheckboxOffTex</t>
   </si>
   <si>
     <t>完全禁用</t>
   </si>
   <si>
+    <t>checkbox, off</t>
+  </si>
+  <si>
+    <t>会以缩放形式复用至右下角叠加层的开关，如果制作外框则视效不佳
+In game it would be used in scaled down, not recommended to add a outer frame texture</t>
+  </si>
+  <si>
+    <t>Widgets.CheckboxOnTex</t>
+  </si>
+  <si>
+    <t>启用</t>
+  </si>
+  <si>
+    <t>checkbox, on</t>
+  </si>
+  <si>
     <t>会以缩放形式复用至右下角叠加层的开关，如果制作外框则视效不佳</t>
   </si>
   <si>
-    <t>Widgets.CheckboxOnTex</t>
-  </si>
-  <si>
-    <t>启用</t>
-  </si>
-  <si>
     <t>Widgets.CheckboxPartialTex</t>
   </si>
   <si>
     <t>部分启用</t>
   </si>
   <si>
-    <t>WidgetsWork.WorkBoxBG_Awful</t>
-  </si>
-  <si>
-    <t>指派-糟糕</t>
-  </si>
-  <si>
-    <t>跳过</t>
-  </si>
-  <si>
-    <t>WidgetsWork.WorkBoxBG_Bad</t>
-  </si>
-  <si>
-    <t>指派-差</t>
-  </si>
-  <si>
-    <t>WidgetsWork.WorkBoxBG_Excellent</t>
-  </si>
-  <si>
-    <t>指派-优秀</t>
-  </si>
-  <si>
-    <t>WidgetsWork.WorkBoxBG_Mid</t>
-  </si>
-  <si>
-    <t>指派-一般</t>
+    <t>checkbox, partial on</t>
   </si>
   <si>
     <t>WidgetsWork.WorkBoxCheckTex</t>
@@ -390,10 +456,7 @@
     <t>指派-打勾</t>
   </si>
   <si>
-    <t>WidgetsWork.WorkBoxOverlay_Warning</t>
-  </si>
-  <si>
-    <t>指派-警告</t>
+    <t>work assgin, check sign</t>
   </si>
   <si>
     <t>SkillUI.PassionMajorIcon</t>
@@ -402,6 +465,9 @@
     <t>双火</t>
   </si>
   <si>
+    <t>major passion, double fire</t>
+  </si>
+  <si>
     <t>后续迭代</t>
   </si>
   <si>
@@ -411,19 +477,29 @@
     <t>单火</t>
   </si>
   <si>
+    <t>minor passion, single fire</t>
+  </si>
+  <si>
     <t>TexButton.CloseXBig</t>
   </si>
   <si>
     <t>关闭按钮</t>
   </si>
   <si>
+    <t>common close button</t>
+  </si>
+  <si>
     <t>TexButton.CloseXSmall</t>
   </si>
   <si>
     <t>一般窗口的右上角关闭按钮</t>
   </si>
   <si>
-    <t>鼠标悬停时会变暗</t>
+    <t>common close button, small</t>
+  </si>
+  <si>
+    <t>鼠标悬停时会变暗
+Darken while mouse on it</t>
   </si>
   <si>
     <t>TexButton.ReorderUp</t>
@@ -432,7 +508,11 @@
     <t>订单窗口右上角-前一个</t>
   </si>
   <si>
-    <t>待验证，可能通过翻转使用，鼠标悬停时会变暗</t>
+    <t>reorder, up</t>
+  </si>
+  <si>
+    <t>待验证，鼠标悬停时会变暗
+Darken while mouse on it</t>
   </si>
   <si>
     <t>TexButton.ReorderDown</t>
@@ -441,6 +521,9 @@
     <t>订单窗口右上角-后一个</t>
   </si>
   <si>
+    <t>reorder, down</t>
+  </si>
+  <si>
     <t>Widgets.FloatRangeSliderTex</t>
   </si>
   <si>
@@ -450,7 +533,11 @@
     <t>设置最大最小值的滑杆边界</t>
   </si>
   <si>
-    <t>游戏内会翻转使用</t>
+    <t>slider edge, set skill level min-max limit of a bill</t>
+  </si>
+  <si>
+    <t>游戏内会翻转使用
+In game it would be used with horizontal flip</t>
   </si>
   <si>
     <t>TexButton.SelectOverlappingNext</t>
@@ -459,6 +546,9 @@
     <t>当有物品堆叠时，切换显示下一个</t>
   </si>
   <si>
+    <t>select overlapping item</t>
+  </si>
+  <si>
     <t>左侧物品/人物面板右上角按钮</t>
   </si>
   <si>
@@ -468,12 +558,18 @@
     <t>信息按钮</t>
   </si>
   <si>
+    <t>info button</t>
+  </si>
+  <si>
     <t>NA</t>
   </si>
   <si>
     <t>垃圾桶图标，删除消息</t>
   </si>
   <si>
+    <t>bin button, not found yet</t>
+  </si>
+  <si>
     <t>未找到</t>
   </si>
   <si>
@@ -486,13 +582,23 @@
     <t>订单减少</t>
   </si>
   <si>
+    <t>bill minus</t>
+  </si>
+  <si>
+    <t>可能会被缩放使用，不建议制作外框
+In game it would be used in scaled down, not recommended to add a outer frame texture</t>
+  </si>
+  <si>
+    <t>TexButton.Plus</t>
+  </si>
+  <si>
+    <t>订单增加</t>
+  </si>
+  <si>
+    <t>bill add</t>
+  </si>
+  <si>
     <t>可能会被缩放使用，不建议制作外框</t>
-  </si>
-  <si>
-    <t>TexButton.Plus</t>
-  </si>
-  <si>
-    <t>订单增加</t>
   </si>
   <si>
     <t>配置项</t>
@@ -631,7 +737,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -639,14 +745,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -661,24 +759,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -698,8 +781,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -721,16 +805,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -744,6 +828,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,15 +850,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -768,7 +874,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -789,19 +895,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,13 +925,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,13 +1003,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,73 +1063,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,48 +1075,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1063,6 +1169,95 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1081,32 +1276,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1155,8 +1326,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1165,7 +1351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1183,134 +1369,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1344,13 +1530,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1359,10 +1563,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1371,10 +1575,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1383,49 +1587,73 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2225,816 +2453,838 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="35.125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15.25" customWidth="1"/>
     <col min="4" max="4" width="31.5" style="10" customWidth="1"/>
-    <col min="5" max="5" width="20" style="10" customWidth="1"/>
-    <col min="6" max="6" width="47.875" customWidth="1"/>
+    <col min="5" max="5" width="21.625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="20" style="10" customWidth="1"/>
+    <col min="7" max="7" width="47.875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="11" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
-        <v>48</v>
+      <c r="E1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" ht="28.5" spans="1:7">
+      <c r="A2" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" ht="28.5" spans="1:7">
+      <c r="A3" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
+      <c r="C3" s="20" t="s">
         <v>61</v>
       </c>
+      <c r="D3" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" ht="28.5" spans="1:7">
+      <c r="A4" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" ht="42.75" spans="1:7">
+      <c r="A8" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="20"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="13" t="s">
+      <c r="D8" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" ht="28.5" spans="1:7">
+      <c r="A11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" ht="28.5" spans="1:7">
+      <c r="A12" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
+      <c r="D14" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" ht="42.75" spans="1:7">
+      <c r="A18" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" ht="28.5" spans="1:7">
+      <c r="A19" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" ht="42.75" spans="1:7">
+      <c r="A20" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" ht="42.75" spans="1:7">
+      <c r="A21" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" ht="57" spans="1:7">
+      <c r="A22" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" ht="28.5" spans="1:7">
+      <c r="A23" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" ht="28.5" spans="1:7">
+      <c r="A24" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F28" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="13" t="s">
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" ht="28.5" spans="1:7">
+      <c r="A29" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" ht="28.5" spans="1:6">
-      <c r="A22" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" ht="28.5" spans="1:6">
-      <c r="A23" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" ht="28.5" spans="1:6">
-      <c r="A24" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="E28" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B34" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="E35" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" s="33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="E36" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" s="33" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="35" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="E38" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="F38" s="34" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="34" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="37" t="s">
-        <v>150</v>
-      </c>
-      <c r="B40" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="E40" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="F40" s="37" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="D41" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="E41" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="35" t="s">
+      <c r="D29" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="B42" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="36" t="s">
+      <c r="E29" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="E42" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="35" t="s">
-        <v>156</v>
+      <c r="F29" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" ht="28.5" spans="1:7">
+      <c r="A30" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" ht="28.5" spans="1:7">
+      <c r="A31" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" ht="28.5" spans="1:7">
+      <c r="A32" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="43" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="F33" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="F34" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B35" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="E35" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="F35" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="G35" s="48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" ht="42.75" spans="1:7">
+      <c r="A36" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="43" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="49" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="E37" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="F37" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="52" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3062,121 +3312,121 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>160</v>
+        <v>193</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>161</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>170</v>
+        <v>203</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>173</v>
+        <v>206</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>182</v>
+        <v>215</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -3184,7 +3434,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3192,7 +3442,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>184</v>
+        <v>217</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3200,7 +3450,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>

</xml_diff>